<commit_message>
update solve file for problem of 2 week
</commit_message>
<xml_diff>
--- a/dojinyou/code_2week/CheckListForm_2week.xlsx
+++ b/dojinyou/code_2week/CheckListForm_2week.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\유도진\Dropbox\MJU\Coin\2.study\21_1\Study-21-1-codingTest\0_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\유도진\Dropbox\MJU\Coin\2.study\21_1\Study-21-1-codingTest\dojinyou\code_2week\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7789B4-475F-4F3F-8D8B-559C4E5BD88E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC990E7-9CB3-4D38-8DA8-B7AEB2CBE47C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="45" windowWidth="14385" windowHeight="15555" xr2:uid="{2683A084-5E1C-45DB-8DAE-141C5F5642CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2683A084-5E1C-45DB-8DAE-141C5F5642CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,6 +196,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,16 +629,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -645,12 +645,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,6 +660,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -675,61 +699,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1047,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA290B9-D938-4FB9-A2F0-C9496544FB19}">
-  <dimension ref="B1:F122"/>
+  <dimension ref="B1:V122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1065,1178 +1071,1308 @@
   <sheetData>
     <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="10" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+    <row r="3" spans="2:6" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="34"/>
-    </row>
-    <row r="7" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="13" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
     </row>
     <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="20"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="22" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="13" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="20"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="22" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="2:6" s="10" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="2:6" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="16" t="s">
+      <c r="F16" s="35">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="33" t="s">
+      <c r="C17" s="26"/>
+      <c r="D17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="30" t="s">
+    <row r="18" spans="2:22" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="34"/>
-    </row>
-    <row r="19" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B19" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="19"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="13" t="s">
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B20" s="15"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="19"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="13" t="s">
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B21" s="15"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="19"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="13" t="s">
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B22" s="15"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="20"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="22" t="s">
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="16"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="21" t="s">
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B24" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="19"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="13" t="s">
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B25" s="15"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="22" t="s">
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24"/>
-    </row>
-    <row r="27" spans="2:6" s="10" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="25" t="s">
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="2:22" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B28" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="26"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="16" t="s">
+      <c r="F28" s="35">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="33" t="s">
+      <c r="C29" s="26"/>
+      <c r="D29" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="30" t="s">
+    <row r="30" spans="2:22" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="34"/>
-    </row>
-    <row r="31" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="18" t="s">
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="29"/>
+    </row>
+    <row r="31" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="27" t="s">
+      <c r="C31" s="32"/>
+      <c r="D31" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="19"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="13" t="s">
+      <c r="E31" s="18"/>
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B32" s="15"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
+      <c r="V32" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="19"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="13" t="s">
+      <c r="B33" s="15"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="19"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="13" t="s">
+      <c r="B34" s="15"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22"/>
     </row>
     <row r="35" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="20"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="22" t="s">
+      <c r="B35" s="16"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="24"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="29"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="19"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="13" t="s">
+      <c r="B37" s="15"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22"/>
     </row>
     <row r="38" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="20"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="22" t="s">
+      <c r="B38" s="16"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="24"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="2:6" ht="7.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="26"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="41" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="33" t="s">
+      <c r="C41" s="26"/>
+      <c r="D41" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="34"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="29"/>
+    </row>
+    <row r="43" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="27" t="s">
+      <c r="C43" s="32"/>
+      <c r="D43" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="29"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="19"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="19"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="13" t="s">
+      <c r="B44" s="15"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="15"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="22"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="19"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="13" t="s">
+      <c r="B45" s="15"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="14"/>
-      <c r="F45" s="15"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="22"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="19"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="13" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="15"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="22"/>
     </row>
     <row r="47" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="20"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="22" t="s">
+      <c r="B47" s="16"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="23"/>
-      <c r="F47" s="24"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="27" t="s">
+      <c r="D48" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="29"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="19"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="19"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="13" t="s">
+      <c r="B49" s="15"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="15"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="20"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="22" t="s">
+      <c r="B50" s="16"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="23"/>
-      <c r="F50" s="24"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="13"/>
     </row>
     <row r="51" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="26"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="53" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="33" t="s">
+      <c r="C53" s="26"/>
+      <c r="D53" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="34"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="18" t="s">
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="29"/>
+    </row>
+    <row r="55" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="27" t="s">
+      <c r="C55" s="32"/>
+      <c r="D55" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="28"/>
-      <c r="F55" s="29"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="19"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B56" s="19"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="13" t="s">
+      <c r="B56" s="15"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="14"/>
-      <c r="F56" s="15"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B57" s="19"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="13" t="s">
+      <c r="B57" s="15"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E57" s="14"/>
-      <c r="F57" s="15"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="22"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="19"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="13" t="s">
+      <c r="B58" s="15"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="14"/>
-      <c r="F58" s="15"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="20"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="22" t="s">
+      <c r="B59" s="16"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E59" s="23"/>
-      <c r="F59" s="24"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="13"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="27" t="s">
+      <c r="D60" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E60" s="28"/>
-      <c r="F60" s="29"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="19"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="19"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="13" t="s">
+      <c r="B61" s="15"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="15"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="22"/>
     </row>
     <row r="62" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="20"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="22" t="s">
+      <c r="B62" s="16"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E62" s="23"/>
-      <c r="F62" s="24"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="13"/>
     </row>
     <row r="63" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="26"/>
+      <c r="C64" s="24"/>
       <c r="D64" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F64" s="2"/>
+      <c r="F64" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="65" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="33" t="s">
+      <c r="C65" s="26"/>
+      <c r="D65" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="31"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="31"/>
-      <c r="F66" s="34"/>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="18" t="s">
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="29"/>
+    </row>
+    <row r="67" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="27" t="s">
+      <c r="C67" s="32"/>
+      <c r="D67" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E67" s="28"/>
-      <c r="F67" s="29"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="19"/>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="19"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="13" t="s">
+      <c r="B68" s="15"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E68" s="14"/>
-      <c r="F68" s="15"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="22"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B69" s="19"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="13" t="s">
+      <c r="B69" s="15"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="15"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="22"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="19"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="13" t="s">
+      <c r="B70" s="15"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="14"/>
-      <c r="F70" s="15"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="22"/>
     </row>
     <row r="71" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="20"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="22" t="s">
+      <c r="B71" s="16"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="23"/>
-      <c r="F71" s="24"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="13"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="27" t="s">
+      <c r="D72" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="28"/>
-      <c r="F72" s="29"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="19"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B73" s="19"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="13" t="s">
+      <c r="B73" s="15"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E73" s="14"/>
-      <c r="F73" s="15"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="22"/>
     </row>
     <row r="74" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="20"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="22" t="s">
+      <c r="B74" s="16"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E74" s="23"/>
-      <c r="F74" s="24"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="13"/>
     </row>
     <row r="75" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B76" s="25" t="s">
+      <c r="B76" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="26"/>
+      <c r="C76" s="24"/>
       <c r="D76" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F76" s="2"/>
+      <c r="F76" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="77" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="17"/>
-      <c r="D77" s="33" t="s">
+      <c r="C77" s="26"/>
+      <c r="D77" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F77" s="4" t="s">
+      <c r="F77" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="30" t="s">
+      <c r="B78" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="34"/>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="18" t="s">
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="29"/>
+    </row>
+    <row r="79" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="27" t="s">
+      <c r="C79" s="32"/>
+      <c r="D79" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E79" s="28"/>
-      <c r="F79" s="29"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="19"/>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B80" s="19"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="13" t="s">
+      <c r="B80" s="15"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E80" s="14"/>
-      <c r="F80" s="15"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="22"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B81" s="19"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="13" t="s">
+      <c r="B81" s="15"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E81" s="14"/>
-      <c r="F81" s="15"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="22"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B82" s="19"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="13" t="s">
+      <c r="B82" s="15"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E82" s="14"/>
-      <c r="F82" s="15"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="22"/>
     </row>
     <row r="83" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="20"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="22" t="s">
+      <c r="B83" s="16"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E83" s="23"/>
-      <c r="F83" s="24"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="13"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B84" s="21" t="s">
+      <c r="B84" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C84" s="1"/>
-      <c r="D84" s="27" t="s">
+      <c r="D84" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E84" s="28"/>
-      <c r="F84" s="29"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="19"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B85" s="19"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="13" t="s">
+      <c r="B85" s="15"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E85" s="14"/>
-      <c r="F85" s="15"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="22"/>
     </row>
     <row r="86" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="20"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="22" t="s">
+      <c r="B86" s="16"/>
+      <c r="C86" s="34"/>
+      <c r="D86" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E86" s="23"/>
-      <c r="F86" s="24"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="13"/>
     </row>
     <row r="87" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B88" s="25" t="s">
+      <c r="B88" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C88" s="26"/>
+      <c r="C88" s="24"/>
       <c r="D88" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F88" s="2"/>
+      <c r="F88" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="89" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="33" t="s">
+      <c r="C89" s="26"/>
+      <c r="D89" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E89" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="F89" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="30" t="s">
+      <c r="B90" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C90" s="31"/>
-      <c r="D90" s="31"/>
-      <c r="E90" s="31"/>
-      <c r="F90" s="34"/>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B91" s="18" t="s">
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="29"/>
+    </row>
+    <row r="91" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="27" t="s">
+      <c r="C91" s="32"/>
+      <c r="D91" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E91" s="28"/>
-      <c r="F91" s="29"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="19"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B92" s="19"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="13" t="s">
+      <c r="B92" s="15"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E92" s="14"/>
-      <c r="F92" s="15"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="22"/>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B93" s="19"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="13" t="s">
+      <c r="B93" s="15"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E93" s="14"/>
-      <c r="F93" s="15"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="22"/>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B94" s="19"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="13" t="s">
+      <c r="B94" s="15"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E94" s="14"/>
-      <c r="F94" s="15"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="22"/>
     </row>
     <row r="95" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="20"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="22" t="s">
+      <c r="B95" s="16"/>
+      <c r="C95" s="34"/>
+      <c r="D95" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E95" s="23"/>
-      <c r="F95" s="24"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="13"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B96" s="21" t="s">
+      <c r="B96" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C96" s="1"/>
-      <c r="D96" s="27" t="s">
+      <c r="D96" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E96" s="28"/>
-      <c r="F96" s="29"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="19"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="19"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="13" t="s">
+      <c r="B97" s="15"/>
+      <c r="C97" s="33"/>
+      <c r="D97" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E97" s="14"/>
-      <c r="F97" s="15"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="22"/>
     </row>
     <row r="98" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="20"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="22" t="s">
+      <c r="B98" s="16"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E98" s="23"/>
-      <c r="F98" s="24"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="13"/>
     </row>
     <row r="99" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B100" s="25" t="s">
+      <c r="B100" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C100" s="26"/>
+      <c r="C100" s="24"/>
       <c r="D100" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F100" s="2"/>
+      <c r="F100" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="101" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="16" t="s">
+      <c r="B101" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C101" s="17"/>
-      <c r="D101" s="33" t="s">
+      <c r="C101" s="26"/>
+      <c r="D101" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E101" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F101" s="4" t="s">
+      <c r="F101" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="102" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="30" t="s">
+      <c r="B102" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="31"/>
-      <c r="D102" s="31"/>
-      <c r="E102" s="31"/>
-      <c r="F102" s="34"/>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B103" s="18" t="s">
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="29"/>
+    </row>
+    <row r="103" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="27" t="s">
+      <c r="C103" s="32"/>
+      <c r="D103" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E103" s="28"/>
-      <c r="F103" s="29"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="19"/>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B104" s="19"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="13" t="s">
+      <c r="B104" s="15"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E104" s="14"/>
-      <c r="F104" s="15"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="22"/>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B105" s="19"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="13" t="s">
+      <c r="B105" s="15"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E105" s="14"/>
-      <c r="F105" s="15"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="22"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B106" s="19"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="13" t="s">
+      <c r="B106" s="15"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E106" s="14"/>
-      <c r="F106" s="15"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="22"/>
     </row>
     <row r="107" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="20"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="22" t="s">
+      <c r="B107" s="16"/>
+      <c r="C107" s="34"/>
+      <c r="D107" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E107" s="23"/>
-      <c r="F107" s="24"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="13"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B108" s="21" t="s">
+      <c r="B108" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C108" s="1"/>
-      <c r="D108" s="27" t="s">
+      <c r="D108" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E108" s="28"/>
-      <c r="F108" s="29"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="19"/>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B109" s="19"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="13" t="s">
+      <c r="B109" s="15"/>
+      <c r="C109" s="33"/>
+      <c r="D109" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E109" s="14"/>
-      <c r="F109" s="15"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="22"/>
     </row>
     <row r="110" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B110" s="20"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="22" t="s">
+      <c r="B110" s="16"/>
+      <c r="C110" s="34"/>
+      <c r="D110" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E110" s="23"/>
-      <c r="F110" s="24"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="13"/>
     </row>
     <row r="111" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="112" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B112" s="25" t="s">
+      <c r="B112" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C112" s="26"/>
+      <c r="C112" s="24"/>
       <c r="D112" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F112" s="2"/>
+      <c r="F112" s="35">
+        <v>44267</v>
+      </c>
     </row>
     <row r="113" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B113" s="16" t="s">
+      <c r="B113" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C113" s="17"/>
-      <c r="D113" s="33" t="s">
+      <c r="C113" s="26"/>
+      <c r="D113" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E113" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F113" s="4" t="s">
+      <c r="F113" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="114" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B114" s="30" t="s">
+      <c r="B114" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="31"/>
-      <c r="D114" s="31"/>
-      <c r="E114" s="31"/>
-      <c r="F114" s="34"/>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B115" s="18" t="s">
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28"/>
+      <c r="F114" s="29"/>
+    </row>
+    <row r="115" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C115" s="6"/>
-      <c r="D115" s="27" t="s">
+      <c r="C115" s="32"/>
+      <c r="D115" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E115" s="28"/>
-      <c r="F115" s="29"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="19"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B116" s="19"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="13" t="s">
+      <c r="B116" s="15"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E116" s="14"/>
-      <c r="F116" s="15"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="22"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B117" s="19"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="13" t="s">
+      <c r="B117" s="15"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E117" s="14"/>
-      <c r="F117" s="15"/>
+      <c r="E117" s="21"/>
+      <c r="F117" s="22"/>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B118" s="19"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="13" t="s">
+      <c r="B118" s="15"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E118" s="14"/>
-      <c r="F118" s="15"/>
+      <c r="E118" s="21"/>
+      <c r="F118" s="22"/>
     </row>
     <row r="119" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="20"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="22" t="s">
+      <c r="B119" s="16"/>
+      <c r="C119" s="34"/>
+      <c r="D119" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E119" s="23"/>
-      <c r="F119" s="24"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="13"/>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B120" s="21" t="s">
+      <c r="B120" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C120" s="1"/>
-      <c r="D120" s="27" t="s">
+      <c r="D120" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E120" s="28"/>
-      <c r="F120" s="29"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="19"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B121" s="19"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="13" t="s">
+      <c r="B121" s="15"/>
+      <c r="C121" s="33"/>
+      <c r="D121" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E121" s="14"/>
-      <c r="F121" s="15"/>
+      <c r="E121" s="21"/>
+      <c r="F121" s="22"/>
     </row>
     <row r="122" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="20"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="22" t="s">
+      <c r="B122" s="16"/>
+      <c r="C122" s="34"/>
+      <c r="D122" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E122" s="23"/>
-      <c r="F122" s="24"/>
+      <c r="E122" s="12"/>
+      <c r="F122" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:B107"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:B119"/>
+    <mergeCell ref="D108:F108"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D115:F115"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="D109:F109"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D67:F67"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="D24:F24"/>
@@ -2261,113 +2397,6 @@
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="D98:F98"/>
-    <mergeCell ref="D97:F97"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D108:F108"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="D115:F115"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="D109:F109"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:B119"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:B107"/>
-    <mergeCell ref="B96:B98"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D43:F43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2383,5 +2412,6 @@
     <hyperlink ref="D5" r:id="rId10" xr:uid="{DE7CAFCB-44D3-423C-B1DA-8DCE489C260B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>